<commit_message>
Version 5 of Tables-FINAL
</commit_message>
<xml_diff>
--- a/Tables for Poster.xlsx
+++ b/Tables for Poster.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hayde\Documents\GitHub\FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EAFC50A-F79F-4149-945C-D72AF9A6F8CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D533614A-4943-4AE7-AC19-83E5779D2518}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="7608" windowWidth="17280" windowHeight="8964" xr2:uid="{C42AB55C-FE8C-492C-9431-47117B25D62C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C42AB55C-FE8C-492C-9431-47117B25D62C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="16">
   <si>
     <t>Gene ID</t>
   </si>
@@ -75,13 +75,42 @@
   </si>
   <si>
     <t xml:space="preserve">Msex2.10735 </t>
+  </si>
+  <si>
+    <t>Midgut</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Table 1. Top three genes experiencing the greatest change in expression within the head, gut and fat tissue of </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Manduca sexta</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> between the 5th instar and adult life stage. Positive values under Change in Expression Level indicate an increase in expression level in the adult stage while negative values indicate a decrease in expression level.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,6 +123,14 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -111,13 +148,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor rgb="FFF3AA79"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor rgb="FFFDCDFB"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -163,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -192,53 +229,56 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -246,6 +286,15 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFDCDFB"/>
+      <color rgb="FFF3AA79"/>
+      <color rgb="FFDF7413"/>
+      <color rgb="FFFFDD7D"/>
+      <color rgb="FF503B00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -556,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02730869-3857-4066-9A71-D32429F83B27}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -844,24 +893,24 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C23" s="10">
         <v>3602.6129999999998</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D23" s="10">
         <v>75574.228000000003</v>
       </c>
-      <c r="E23" s="11">
+      <c r="E23" s="10">
         <v>71971.615000000005</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="12"/>
+      <c r="A24" s="24"/>
       <c r="B24" s="3" t="s">
         <v>10</v>
       </c>
@@ -876,7 +925,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="13"/>
+      <c r="A25" s="25"/>
       <c r="B25" s="5" t="s">
         <v>11</v>
       </c>
@@ -891,24 +940,24 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C26" s="10">
         <v>43171.26</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D26" s="10">
         <v>2205.5520000000001</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E26" s="10">
         <v>-40965.707999999999</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="13"/>
+      <c r="A27" s="25"/>
       <c r="B27" s="5" t="s">
         <v>10</v>
       </c>
@@ -980,12 +1029,14 @@
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
+    <row r="32" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>
@@ -1015,40 +1066,40 @@
       <c r="A35" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="15">
+      <c r="C35" s="22">
         <v>74964.413</v>
       </c>
-      <c r="D35" s="15">
+      <c r="D35" s="22">
         <v>439.17200000000003</v>
       </c>
-      <c r="E35" s="15">
+      <c r="E35" s="22">
         <v>-7425.241</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="17">
+      <c r="C36" s="21">
         <v>3602.6129999999998</v>
       </c>
-      <c r="D36" s="17">
+      <c r="D36" s="21">
         <v>75574.228000000003</v>
       </c>
-      <c r="E36" s="17">
+      <c r="E36" s="21">
         <v>71971.615000000005</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="12"/>
+      <c r="A37" s="24"/>
       <c r="B37" s="18" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C37" s="18">
         <v>17344.096000000001</v>
@@ -1061,49 +1112,49 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="13"/>
-      <c r="B38" s="19" t="s">
+      <c r="A38" s="25"/>
+      <c r="B38" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C38" s="19">
+      <c r="C38" s="11">
         <v>68477.053</v>
       </c>
-      <c r="D38" s="19">
+      <c r="D38" s="11">
         <v>237523.435</v>
       </c>
-      <c r="E38" s="19">
+      <c r="E38" s="11">
         <v>169046.38200000001</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="9" t="s">
+      <c r="A39" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="17">
+      <c r="C39" s="21">
         <v>43171.26</v>
       </c>
-      <c r="D39" s="17">
+      <c r="D39" s="21">
         <v>2205.5520000000001</v>
       </c>
-      <c r="E39" s="17">
+      <c r="E39" s="21">
         <v>-40965.707999999999</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="13"/>
-      <c r="B40" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C40" s="21">
+      <c r="A40" s="25"/>
+      <c r="B40" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="15">
         <v>43268.046000000002</v>
       </c>
-      <c r="D40" s="21">
+      <c r="D40" s="15">
         <v>3490.07</v>
       </c>
-      <c r="E40" s="21">
+      <c r="E40" s="15">
         <v>-39777.976000000002</v>
       </c>
     </row>
@@ -1111,16 +1162,16 @@
       <c r="A41" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B41" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" s="23">
+      <c r="B41" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="17">
         <v>118.13800000000001</v>
       </c>
-      <c r="D41" s="23">
+      <c r="D41" s="17">
         <v>82120.42</v>
       </c>
-      <c r="E41" s="23">
+      <c r="E41" s="17">
         <v>82002.282000000007</v>
       </c>
     </row>
@@ -1128,16 +1179,16 @@
       <c r="A42" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B42" s="24" t="s">
+      <c r="B42" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C42" s="25">
+      <c r="C42" s="13">
         <v>68823.61</v>
       </c>
-      <c r="D42" s="25">
+      <c r="D42" s="13">
         <v>26.09</v>
       </c>
-      <c r="E42" s="25">
+      <c r="E42" s="13">
         <v>-68797.52</v>
       </c>
     </row>
@@ -1145,25 +1196,26 @@
       <c r="A43" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C43" s="25">
+      <c r="C43" s="13">
         <v>27176.113000000001</v>
       </c>
-      <c r="D43" s="25">
+      <c r="D43" s="13">
         <v>9.57</v>
       </c>
-      <c r="E43" s="25">
+      <c r="E43" s="13">
         <v>-27166.543000000001</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="A36:A38"/>
     <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A32:E32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Table with Protien, Function, Expression Levels, in final order
</commit_message>
<xml_diff>
--- a/Tables for Poster.xlsx
+++ b/Tables for Poster.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hayde\Documents\GitHub\FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D533614A-4943-4AE7-AC19-83E5779D2518}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179A65F0-B1D7-4354-8699-6902F2FFEFFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C42AB55C-FE8C-492C-9431-47117B25D62C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="29">
   <si>
     <t>Gene ID</t>
   </si>
@@ -105,12 +105,72 @@
       <t xml:space="preserve"> between the 5th instar and adult life stage. Positive values under Change in Expression Level indicate an increase in expression level in the adult stage while negative values indicate a decrease in expression level.</t>
     </r>
   </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Ejaculatory bulb-specific protein 3-like</t>
+  </si>
+  <si>
+    <t>Chemosensation, tissue remodeling, host defense</t>
+  </si>
+  <si>
+    <t>Uncharacterized</t>
+  </si>
+  <si>
+    <t>ATP synthase F0 subunit 6 (mitochondrion)</t>
+  </si>
+  <si>
+    <t>ATP synthesis, oxidative phosphorylation</t>
+  </si>
+  <si>
+    <t>basic juvenile hormone-suppressible protein 2-like</t>
+  </si>
+  <si>
+    <t>Energy storage</t>
+  </si>
+  <si>
+    <t>basic juvenile hormone-suppressible protein 1-like</t>
+  </si>
+  <si>
+    <t>Protein Name</t>
+  </si>
+  <si>
+    <t>Basic juvenile hormone-suppressible protein 2-like</t>
+  </si>
+  <si>
+    <t>Basic juvenile hormone-suppressible protein 1-like</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Table 1. Top three genes experiencing the greatest change in expression within the head, gut and fat tissue of </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Manduca sexta</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> between the 5th instar and adult life stage. Positive values under Change in Expression Level indicate an increase in expression level in the adult stage while negative values indicate a decrease in expression level. The protien name and function associated with each gene ID were identified from a BLAST analysis</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,6 +191,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -200,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -268,6 +335,9 @@
     <xf numFmtId="2" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -278,6 +348,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -603,19 +700,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02730869-3857-4066-9A71-D32429F83B27}">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="J61" sqref="J61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.44140625" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" customWidth="1"/>
-    <col min="3" max="3" width="19.21875" customWidth="1"/>
+    <col min="2" max="2" width="24.77734375" customWidth="1"/>
+    <col min="3" max="3" width="32.5546875" customWidth="1"/>
     <col min="4" max="4" width="24.21875" customWidth="1"/>
     <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
@@ -893,7 +992,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="24" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="9" t="s">
@@ -910,7 +1009,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="24"/>
+      <c r="A24" s="25"/>
       <c r="B24" s="3" t="s">
         <v>10</v>
       </c>
@@ -925,7 +1024,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="25"/>
+      <c r="A25" s="26"/>
       <c r="B25" s="5" t="s">
         <v>11</v>
       </c>
@@ -940,7 +1039,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="24" t="s">
         <v>8</v>
       </c>
       <c r="B26" s="9" t="s">
@@ -957,7 +1056,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="25"/>
+      <c r="A27" s="26"/>
       <c r="B27" s="5" t="s">
         <v>10</v>
       </c>
@@ -1030,22 +1129,22 @@
       <c r="E31" s="7"/>
     </row>
     <row r="32" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="26" t="s">
+      <c r="A32" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>0</v>
       </c>
@@ -1061,8 +1160,14 @@
       <c r="E34" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F34" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="G34" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>5</v>
       </c>
@@ -1078,9 +1183,15 @@
       <c r="E35" s="22">
         <v>-7425.241</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="23" t="s">
+      <c r="F35" t="s">
+        <v>17</v>
+      </c>
+      <c r="G35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="24" t="s">
         <v>7</v>
       </c>
       <c r="B36" s="20" t="s">
@@ -1095,9 +1206,13 @@
       <c r="E36" s="21">
         <v>71971.615000000005</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="24"/>
+      <c r="F36" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G36" s="28"/>
+    </row>
+    <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="25"/>
       <c r="B37" s="18" t="s">
         <v>14</v>
       </c>
@@ -1110,9 +1225,11 @@
       <c r="E37" s="18">
         <v>45603.953999999998</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="25"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="28"/>
+    </row>
+    <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="26"/>
       <c r="B38" s="11" t="s">
         <v>11</v>
       </c>
@@ -1125,9 +1242,11 @@
       <c r="E38" s="11">
         <v>169046.38200000001</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="23" t="s">
+      <c r="F38" s="28"/>
+      <c r="G38" s="28"/>
+    </row>
+    <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="24" t="s">
         <v>8</v>
       </c>
       <c r="B39" s="20" t="s">
@@ -1142,9 +1261,15 @@
       <c r="E39" s="21">
         <v>-40965.707999999999</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="25"/>
+      <c r="F39" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="G39" s="28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="26"/>
       <c r="B40" s="14" t="s">
         <v>14</v>
       </c>
@@ -1157,8 +1282,10 @@
       <c r="E40" s="15">
         <v>-39777.976000000002</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F40" s="28"/>
+      <c r="G40" s="28"/>
+    </row>
+    <row r="41" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>9</v>
       </c>
@@ -1174,8 +1301,11 @@
       <c r="E41" s="17">
         <v>82002.282000000007</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F41" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>12</v>
       </c>
@@ -1191,8 +1321,14 @@
       <c r="E42" s="13">
         <v>-68797.52</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F42" t="s">
+        <v>22</v>
+      </c>
+      <c r="G42" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>13</v>
       </c>
@@ -1208,16 +1344,257 @@
       <c r="E43" s="13">
         <v>-27166.543000000001</v>
       </c>
+      <c r="F43" t="s">
+        <v>24</v>
+      </c>
+      <c r="G43" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="23.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="1:7" ht="10.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B53" s="27"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="27"/>
+      <c r="E53" s="27"/>
+      <c r="F53" s="27"/>
+      <c r="G53" s="27"/>
+    </row>
+    <row r="54" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C54" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A55" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D55" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55" s="22">
+        <v>74964.413</v>
+      </c>
+      <c r="F55" s="22">
+        <v>439.17200000000003</v>
+      </c>
+      <c r="G55" s="22">
+        <v>-7425.241</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A56" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C56" s="31"/>
+      <c r="D56" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56" s="21">
+        <v>3602.6129999999998</v>
+      </c>
+      <c r="F56" s="21">
+        <v>75574.228000000003</v>
+      </c>
+      <c r="G56" s="21">
+        <v>71971.615000000005</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="25"/>
+      <c r="B57" s="32"/>
+      <c r="C57" s="32"/>
+      <c r="D57" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E57" s="18">
+        <v>17344.096000000001</v>
+      </c>
+      <c r="F57" s="18">
+        <v>62948.05</v>
+      </c>
+      <c r="G57" s="18">
+        <v>45603.953999999998</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="26"/>
+      <c r="B58" s="33"/>
+      <c r="C58" s="33"/>
+      <c r="D58" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" s="11">
+        <v>68477.053</v>
+      </c>
+      <c r="F58" s="11">
+        <v>237523.435</v>
+      </c>
+      <c r="G58" s="11">
+        <v>169046.38200000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A59" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B59" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C59" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D59" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E59" s="21">
+        <v>43171.26</v>
+      </c>
+      <c r="F59" s="21">
+        <v>2205.5520000000001</v>
+      </c>
+      <c r="G59" s="21">
+        <v>-40965.707999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A60" s="26"/>
+      <c r="B60" s="26"/>
+      <c r="C60" s="26"/>
+      <c r="D60" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E60" s="15">
+        <v>43268.046000000002</v>
+      </c>
+      <c r="F60" s="15">
+        <v>3490.07</v>
+      </c>
+      <c r="G60" s="15">
+        <v>-39777.976000000002</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B61" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C61" s="34"/>
+      <c r="D61" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E61" s="17">
+        <v>118.13800000000001</v>
+      </c>
+      <c r="F61" s="17">
+        <v>82120.42</v>
+      </c>
+      <c r="G61" s="17">
+        <v>82002.282000000007</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" s="13">
+        <v>68823.61</v>
+      </c>
+      <c r="F62" s="13">
+        <v>26.09</v>
+      </c>
+      <c r="G62" s="13">
+        <v>-68797.52</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E63" s="13">
+        <v>27176.113000000001</v>
+      </c>
+      <c r="F63" s="13">
+        <v>9.57</v>
+      </c>
+      <c r="G63" s="13">
+        <v>-27166.543000000001</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="15">
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="A53:G53"/>
+    <mergeCell ref="F36:G38"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="B56:C58"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="A36:A38"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="A32:E32"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F42" r:id="rId1" location="alnHdr_XP_022823233" tooltip="Go to alignment for basic juvenile hormone-suppressible protein 2 [Spodoptera litura]" display="https://blast.ncbi.nlm.nih.gov/Blast.cgi - alnHdr_XP_022823233" xr:uid="{DB7A7A37-316E-4099-AF37-C2C19BA9C3C1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967293" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>